<commit_message>
changed date from str to datetime added new qualidications (black list and done) behaviour table appens mode behaviour table process b exp_id and not user_id
</commit_message>
<xml_diff>
--- a/resources/reports/feedback_all_prefix_1_limit_5.xlsx
+++ b/resources/reports/feedback_all_prefix_1_limit_5.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="151">
   <si>
     <t>sequence</t>
   </si>
@@ -1013,7 +1013,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
@@ -1022,6 +1022,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -6348,7 +6349,7 @@
   <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="Z31" sqref="Z31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6949,8 +6950,22 @@
         <v>1</v>
       </c>
       <c r="Y10">
-        <f t="shared" si="1"/>
+        <f>SUM(B10:D10)</f>
         <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="S12" t="s">
+        <v>0</v>
+      </c>
+      <c r="T12" t="s">
+        <v>1</v>
+      </c>
+      <c r="U12" t="s">
+        <v>2</v>
+      </c>
+      <c r="V12" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -6999,6 +7014,25 @@
       <c r="P13">
         <v>0</v>
       </c>
+      <c r="S13" t="s">
+        <v>25</v>
+      </c>
+      <c r="T13">
+        <f>B13/(1-B13)</f>
+        <v>1.0833333333333335</v>
+      </c>
+      <c r="U13">
+        <f t="shared" ref="U13:W13" si="2">C13/(1-C13)</f>
+        <v>0.35135135135135137</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="2"/>
+        <v>2.0408163265306124E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -7046,6 +7080,25 @@
       <c r="P14">
         <v>0</v>
       </c>
+      <c r="S14" t="s">
+        <v>21</v>
+      </c>
+      <c r="T14" s="2">
+        <f t="shared" ref="T14:T21" si="3">B14/(1-B14)</f>
+        <v>0.48571428571428366</v>
+      </c>
+      <c r="U14" s="2">
+        <f t="shared" ref="U14:U21" si="4">C14/(1-C14)</f>
+        <v>0.79310344827586121</v>
+      </c>
+      <c r="V14" s="2">
+        <f t="shared" ref="V14:V21" si="5">D14/(1-D14)</f>
+        <v>0.29999999999999871</v>
+      </c>
+      <c r="W14" s="2">
+        <f t="shared" ref="W14:W21" si="6">E14/(1-E14)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -7093,8 +7146,27 @@
       <c r="P15">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S15" t="s">
+        <v>24</v>
+      </c>
+      <c r="T15" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25641025641025605</v>
+      </c>
+      <c r="U15" s="6">
+        <f t="shared" si="4"/>
+        <v>0.68965517241379182</v>
+      </c>
+      <c r="V15" s="6">
+        <f t="shared" si="5"/>
+        <v>0.53124999999999989</v>
+      </c>
+      <c r="W15" s="6">
+        <f t="shared" si="6"/>
+        <v>4.2553191489361653E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -7140,8 +7212,31 @@
       <c r="P17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S17" t="s">
+        <v>23</v>
+      </c>
+      <c r="T17" s="2">
+        <f t="shared" si="3"/>
+        <v>0.43243243243243207</v>
+      </c>
+      <c r="U17" s="2">
+        <f t="shared" si="4"/>
+        <v>0.82758620689655071</v>
+      </c>
+      <c r="V17" s="2">
+        <f t="shared" si="5"/>
+        <v>0.29268292682926722</v>
+      </c>
+      <c r="W17" s="2">
+        <f t="shared" si="6"/>
+        <v>1.9230769230769138E-2</v>
+      </c>
+      <c r="Y17" s="2">
+        <f>T17/T14</f>
+        <v>0.890302066772658</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -7187,9 +7282,32 @@
       <c r="P18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S18" t="s">
+        <v>27</v>
+      </c>
+      <c r="T18" s="6">
+        <f t="shared" si="3"/>
+        <v>0.2682926829268284</v>
+      </c>
+      <c r="U18" s="6">
+        <f t="shared" si="4"/>
+        <v>0.52941176470588203</v>
+      </c>
+      <c r="V18" s="6">
+        <f t="shared" si="5"/>
+        <v>0.79310344827586121</v>
+      </c>
+      <c r="W18" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X18" s="6">
+        <f>V18/V15</f>
+        <v>1.4929006085192684</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -7235,8 +7353,31 @@
       <c r="P20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S20" t="s">
+        <v>18</v>
+      </c>
+      <c r="T20" s="2">
+        <f t="shared" si="3"/>
+        <v>0.68421052631578949</v>
+      </c>
+      <c r="U20" s="2">
+        <f t="shared" si="4"/>
+        <v>0.6</v>
+      </c>
+      <c r="V20" s="2">
+        <f t="shared" si="5"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="W20" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y20" s="2">
+        <f>T20/T14</f>
+        <v>1.4086687306501608</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -7282,8 +7423,37 @@
       <c r="P21">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S21" t="s">
+        <v>20</v>
+      </c>
+      <c r="T21" s="6">
+        <f t="shared" si="3"/>
+        <v>0.269230769230769</v>
+      </c>
+      <c r="U21" s="6">
+        <f t="shared" si="4"/>
+        <v>0.269230769230769</v>
+      </c>
+      <c r="V21" s="6">
+        <f t="shared" si="5"/>
+        <v>1.0624999999999996</v>
+      </c>
+      <c r="W21" s="6">
+        <f t="shared" si="6"/>
+        <v>6.4516129032258049E-2</v>
+      </c>
+      <c r="X21" s="6">
+        <f>V21/V15</f>
+        <v>1.9999999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X22">
+        <f>LN(X21)</f>
+        <v>0.69314718055994506</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -7318,7 +7488,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -7353,7 +7523,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -7388,7 +7558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -7423,7 +7593,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -7458,7 +7628,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -7493,7 +7663,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -7609,7 +7779,7 @@
   <dimension ref="A1:AA34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E10"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8103,12 +8273,6 @@
         <v>15.232323232323232</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="V14">
-        <f>_xlfn.CHISQ.TEST(W9:Y9,W3:Y3)</f>
-        <v>1.5880081601077095E-2</v>
-      </c>
-    </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="I15" t="s">
         <v>0</v>
@@ -8447,8 +8611,8 @@
     </row>
     <row r="34" spans="19:24" x14ac:dyDescent="0.25">
       <c r="X34">
-        <f>_xlfn.CHISQ.TEST(T25:V25,T26:V26)</f>
-        <v>5.8566326435130424E-4</v>
+        <f>_xlfn.CHISQ.TEST(T25:V26,T32:V33)</f>
+        <v>0.74935874159222793</v>
       </c>
     </row>
   </sheetData>

</xml_diff>